<commit_message>
implemented updateExternalReferences on the SpreadsheetDataSource
</commit_message>
<xml_diff>
--- a/test/extref.xlsx
+++ b/test/extref.xlsx
@@ -4,18 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="foo" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="bar" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>text</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,8 +59,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,12 +80,44 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val=""/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
       <sheetName val="bar"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="bar"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="bar"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -379,15 +422,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D7:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="e">
-        <f>[1]bar!$A$1</f>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="e">
+        <f>+[1]bar!$C$7</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="e">
+        <f>+[2]bar!$C$8</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="e">
+        <f>+[3]bar!$C$9</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -398,12 +455,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f>SUM(A1:A3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: unescape source sheet names on update external references. poi also seems to have issues with this as evaluating all cells with external references formulas containing escaped sheet names fails with an exception.
</commit_message>
<xml_diff>
--- a/test/extref.xlsx
+++ b/test/extref.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="foo" sheetId="2" r:id="rId2"/>
     <sheet name="bar" sheetId="3" r:id="rId3"/>
+    <sheet name="O'Brien's Sales" sheetId="4" r:id="rId4"/>
+    <sheet name="O'Brien's" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
@@ -115,6 +119,38 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="bar"/>
+      <sheetName val="source |'!@#$%^&amp;()_-=+"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="bar"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="O'Brien's"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -425,7 +461,7 @@
   <dimension ref="D7:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -492,4 +528,68 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f>SUM(A1:A3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="e">
+        <f>[4]bar!A1</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="e">
+        <f>'[5]O''Brien''s'!A1</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Unescaping external reference filenames.
</commit_message>
<xml_diff>
--- a/test/extref.xlsx
+++ b/test/extref.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
@@ -19,8 +19,9 @@
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -76,6 +77,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -154,6 +158,25 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="areaBelow50_ordered"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="28">
+          <cell r="Z28">
+            <v>0.3</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -202,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,10 +555,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,6 +590,12 @@
       <c r="E4" t="e">
         <f>'[5]O''Brien''s'!A1</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>[6]areaBelow50_ordered!$Z$28</f>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>